<commit_message>
Fixed unwanteed YoY Selections
</commit_message>
<xml_diff>
--- a/0_0_Data/3_Naive_Forecaster_Data/1_YoY_Forecast_Vectors/forecast_series_yoy_AR2_50_6_full.xlsx
+++ b/0_0_Data/3_Naive_Forecaster_Data/1_YoY_Forecast_Vectors/forecast_series_yoy_AR2_50_6_full.xlsx
@@ -392,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,536 +417,2407 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2">
-        <v>40221</v>
+        <v>32508</v>
       </c>
       <c r="B2">
-        <v>2010</v>
+        <v>1988</v>
       </c>
       <c r="C2">
-        <v>0.9288791585305711</v>
+        <v>3.194969449935003</v>
       </c>
       <c r="D2">
-        <v>2011</v>
+        <v>1989</v>
+      </c>
+      <c r="E2">
+        <v>2.654510774528207</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2">
-        <v>40310</v>
+        <v>32598</v>
       </c>
       <c r="B3">
-        <v>2010</v>
+        <v>1989</v>
       </c>
       <c r="C3">
-        <v>1.071809041675276</v>
+        <v>3.078003875303725</v>
       </c>
       <c r="D3">
-        <v>2011</v>
-      </c>
-      <c r="E3">
-        <v>0.8342879232527967</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2">
-        <v>40403</v>
+        <v>32689</v>
       </c>
       <c r="B4">
-        <v>2010</v>
+        <v>1989</v>
       </c>
       <c r="C4">
-        <v>3.577564492651675</v>
+        <v>3.661580277249166</v>
       </c>
       <c r="D4">
-        <v>2011</v>
+        <v>1990</v>
       </c>
       <c r="E4">
-        <v>2.731583858664188</v>
+        <v>2.193258610001214</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2">
-        <v>40494</v>
+        <v>32781</v>
       </c>
       <c r="B5">
-        <v>2010</v>
+        <v>1989</v>
       </c>
       <c r="C5">
-        <v>3.522877896197807</v>
+        <v>3.6938275965265</v>
       </c>
       <c r="D5">
-        <v>2011</v>
+        <v>1990</v>
       </c>
       <c r="E5">
-        <v>2.252953350090348</v>
+        <v>2.191051164767877</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2">
-        <v>40589</v>
+        <v>32873</v>
       </c>
       <c r="B6">
-        <v>2011</v>
+        <v>1989</v>
       </c>
       <c r="C6">
-        <v>2.021953894754303</v>
+        <v>3.85009945173751</v>
       </c>
       <c r="D6">
-        <v>2012</v>
+        <v>1990</v>
+      </c>
+      <c r="E6">
+        <v>2.342799083309055</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2">
-        <v>40676</v>
+        <v>32963</v>
       </c>
       <c r="B7">
-        <v>2011</v>
+        <v>1990</v>
       </c>
       <c r="C7">
-        <v>3.720096369677184</v>
+        <v>2.666162325285693</v>
       </c>
       <c r="D7">
-        <v>2012</v>
-      </c>
-      <c r="E7">
-        <v>1.686787594525496</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2">
-        <v>40771</v>
+        <v>33054</v>
       </c>
       <c r="B8">
-        <v>2011</v>
+        <v>1990</v>
       </c>
       <c r="C8">
-        <v>2.851982935378228</v>
+        <v>4.130619852766437</v>
       </c>
       <c r="D8">
-        <v>2012</v>
+        <v>1991</v>
       </c>
       <c r="E8">
-        <v>1.136030550102829</v>
+        <v>2.272904440822465</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2">
-        <v>40862</v>
+        <v>33146</v>
       </c>
       <c r="B9">
-        <v>2011</v>
+        <v>1990</v>
       </c>
       <c r="C9">
-        <v>3.172593145981373</v>
+        <v>4.360305978402312</v>
       </c>
       <c r="D9">
-        <v>2012</v>
+        <v>1991</v>
       </c>
       <c r="E9">
-        <v>1.460171959067247</v>
+        <v>2.354203638264551</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2">
-        <v>40954</v>
+        <v>33238</v>
       </c>
       <c r="B10">
-        <v>2012</v>
+        <v>1990</v>
       </c>
       <c r="C10">
-        <v>0.613364121638349</v>
+        <v>5.073362306219398</v>
       </c>
       <c r="D10">
-        <v>2013</v>
+        <v>1991</v>
+      </c>
+      <c r="E10">
+        <v>2.977303796668029</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2">
-        <v>41044</v>
+        <v>33328</v>
       </c>
       <c r="B11">
-        <v>2012</v>
+        <v>1991</v>
       </c>
       <c r="C11">
-        <v>1.276650241283095</v>
+        <v>3.912848990577067</v>
       </c>
       <c r="D11">
-        <v>2013</v>
-      </c>
-      <c r="E11">
-        <v>1.19633550657503</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2">
-        <v>41135</v>
+        <v>33419</v>
       </c>
       <c r="B12">
-        <v>2012</v>
+        <v>1991</v>
       </c>
       <c r="C12">
-        <v>1.086563863520862</v>
+        <v>6.364491101711689</v>
       </c>
       <c r="D12">
-        <v>2013</v>
+        <v>1992</v>
       </c>
       <c r="E12">
-        <v>1.06457164149647</v>
+        <v>2.793798186209284</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2">
-        <v>41228</v>
+        <v>33511</v>
       </c>
       <c r="B13">
-        <v>2012</v>
+        <v>1991</v>
       </c>
       <c r="C13">
-        <v>1.075749333634834</v>
+        <v>6.813462808712534</v>
       </c>
       <c r="D13">
-        <v>2013</v>
+        <v>1992</v>
       </c>
       <c r="E13">
-        <v>1.106002658655192</v>
+        <v>2.829294614456113</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2">
-        <v>41319</v>
+        <v>33603</v>
       </c>
       <c r="B14">
-        <v>2013</v>
+        <v>1991</v>
       </c>
       <c r="C14">
-        <v>-0.1408840671955125</v>
+        <v>6.091605135014255</v>
       </c>
       <c r="D14">
-        <v>2014</v>
+        <v>1992</v>
+      </c>
+      <c r="E14">
+        <v>2.066726874661873</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2">
-        <v>41409</v>
+        <v>33694</v>
       </c>
       <c r="B15">
-        <v>2013</v>
+        <v>1992</v>
       </c>
       <c r="C15">
-        <v>-0.03137857138646449</v>
+        <v>2.139879630803643</v>
       </c>
       <c r="D15">
-        <v>2014</v>
-      </c>
-      <c r="E15">
-        <v>0.8494291553396094</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2">
-        <v>41500</v>
+        <v>33785</v>
       </c>
       <c r="B16">
-        <v>2013</v>
+        <v>1992</v>
       </c>
       <c r="C16">
-        <v>0.6094282583182231</v>
+        <v>2.932796654414149</v>
       </c>
       <c r="D16">
-        <v>2014</v>
+        <v>1993</v>
       </c>
       <c r="E16">
-        <v>1.440500538214629</v>
+        <v>2.584450468619459</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2">
-        <v>41592</v>
+        <v>33877</v>
       </c>
       <c r="B17">
-        <v>2013</v>
+        <v>1992</v>
       </c>
       <c r="C17">
-        <v>0.5135943516859198</v>
+        <v>2.494110716709286</v>
       </c>
       <c r="D17">
-        <v>2014</v>
+        <v>1993</v>
       </c>
       <c r="E17">
-        <v>1.304915753449687</v>
+        <v>2.492787484240577</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2">
-        <v>41684</v>
+        <v>33969</v>
       </c>
       <c r="B18">
-        <v>2014</v>
+        <v>1992</v>
       </c>
       <c r="C18">
-        <v>1.408749482567595</v>
+        <v>2.064701871240571</v>
       </c>
       <c r="D18">
-        <v>2015</v>
+        <v>1993</v>
+      </c>
+      <c r="E18">
+        <v>2.112386427028046</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2">
-        <v>41774</v>
+        <v>34059</v>
       </c>
       <c r="B19">
-        <v>2014</v>
+        <v>1993</v>
       </c>
       <c r="C19">
-        <v>2.183348446776856</v>
+        <v>1.549317903069802</v>
       </c>
       <c r="D19">
-        <v>2015</v>
-      </c>
-      <c r="E19">
-        <v>1.476241482808471</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2">
-        <v>41865</v>
+        <v>34150</v>
       </c>
       <c r="B20">
-        <v>2014</v>
+        <v>1993</v>
       </c>
       <c r="C20">
-        <v>1.308305381840369</v>
+        <v>-1.06363680093724</v>
       </c>
       <c r="D20">
-        <v>2015</v>
+        <v>1994</v>
       </c>
       <c r="E20">
-        <v>0.726330085526028</v>
+        <v>2.368493192930488</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2">
-        <v>41957</v>
+        <v>34242</v>
       </c>
       <c r="B21">
-        <v>2014</v>
+        <v>1993</v>
       </c>
       <c r="C21">
-        <v>1.463603839062211</v>
+        <v>-1.124761626679238</v>
       </c>
       <c r="D21">
-        <v>2015</v>
+        <v>1994</v>
       </c>
       <c r="E21">
-        <v>0.7345358670387547</v>
+        <v>2.402262657257404</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2">
-        <v>42048</v>
+        <v>34334</v>
       </c>
       <c r="B22">
-        <v>2015</v>
+        <v>1993</v>
       </c>
       <c r="C22">
-        <v>1.555506802213324</v>
+        <v>-1.000531514043412</v>
       </c>
       <c r="D22">
-        <v>2016</v>
+        <v>1994</v>
+      </c>
+      <c r="E22">
+        <v>2.575999544954621</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2">
-        <v>42137</v>
+        <v>34424</v>
       </c>
       <c r="B23">
-        <v>2015</v>
+        <v>1994</v>
       </c>
       <c r="C23">
-        <v>1.291204709804039</v>
+        <v>1.991768926775084</v>
       </c>
       <c r="D23">
-        <v>2016</v>
-      </c>
-      <c r="E23">
-        <v>1.334784545494694</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2">
-        <v>42230</v>
+        <v>34515</v>
       </c>
       <c r="B24">
-        <v>2015</v>
+        <v>1994</v>
       </c>
       <c r="C24">
-        <v>1.503879794234519</v>
+        <v>2.479893153134016</v>
       </c>
       <c r="D24">
-        <v>2016</v>
+        <v>1995</v>
       </c>
       <c r="E24">
-        <v>1.427154289074717</v>
+        <v>2.567096653116252</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2">
-        <v>42321</v>
+        <v>34607</v>
       </c>
       <c r="B25">
-        <v>2015</v>
+        <v>1994</v>
       </c>
       <c r="C25">
-        <v>1.460561192715071</v>
+        <v>2.993503501929951</v>
       </c>
       <c r="D25">
-        <v>2016</v>
+        <v>1995</v>
       </c>
       <c r="E25">
-        <v>1.316306168565684</v>
+        <v>2.851639473444134</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2">
-        <v>42412</v>
+        <v>34699</v>
       </c>
       <c r="B26">
-        <v>2016</v>
+        <v>1994</v>
       </c>
       <c r="C26">
-        <v>1.211140135558786</v>
+        <v>2.998503002360153</v>
       </c>
       <c r="D26">
-        <v>2017</v>
+        <v>1995</v>
+      </c>
+      <c r="E26">
+        <v>2.954478109176528</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2">
-        <v>42503</v>
+        <v>34789</v>
       </c>
       <c r="B27">
-        <v>2016</v>
+        <v>1995</v>
       </c>
       <c r="C27">
-        <v>1.789277221144991</v>
+        <v>2.923150766105942</v>
       </c>
       <c r="D27">
-        <v>2017</v>
-      </c>
-      <c r="E27">
-        <v>1.517762585655458</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2">
-        <v>42594</v>
+        <v>34880</v>
       </c>
       <c r="B28">
-        <v>2016</v>
+        <v>1995</v>
       </c>
       <c r="C28">
-        <v>1.831409032854858</v>
+        <v>2.432437183852798</v>
       </c>
       <c r="D28">
-        <v>2017</v>
+        <v>1996</v>
       </c>
       <c r="E28">
-        <v>1.455762792597137</v>
+        <v>2.872765583543457</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2">
-        <v>42689</v>
+        <v>34948</v>
       </c>
       <c r="B29">
-        <v>2016</v>
+        <v>1995</v>
       </c>
       <c r="C29">
-        <v>1.71486702353103</v>
+        <v>2.622955649346648</v>
       </c>
       <c r="D29">
-        <v>2017</v>
+        <v>1996</v>
       </c>
       <c r="E29">
-        <v>1.271337706785514</v>
+        <v>2.915653518291639</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2">
-        <v>42780</v>
+        <v>35040</v>
       </c>
       <c r="B30">
-        <v>2017</v>
+        <v>1995</v>
       </c>
       <c r="C30">
-        <v>1.469790059051301</v>
+        <v>2.310325699082871</v>
       </c>
       <c r="D30">
-        <v>2018</v>
+        <v>1996</v>
+      </c>
+      <c r="E30">
+        <v>2.658356052145039</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2">
-        <v>42867</v>
+        <v>35131</v>
       </c>
       <c r="B31">
-        <v>2017</v>
+        <v>1996</v>
       </c>
       <c r="C31">
-        <v>1.816297695264346</v>
+        <v>1.87529243636666</v>
       </c>
       <c r="D31">
-        <v>2018</v>
-      </c>
-      <c r="E31">
-        <v>1.651160881705249</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2">
-        <v>42962</v>
+        <v>35221</v>
       </c>
       <c r="B32">
-        <v>2017</v>
+        <v>1996</v>
       </c>
       <c r="C32">
-        <v>2.141958087655205</v>
+        <v>0.7757377956089551</v>
       </c>
       <c r="D32">
-        <v>2018</v>
+        <v>1997</v>
       </c>
       <c r="E32">
-        <v>1.746314025496809</v>
+        <v>2.610245619887741</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2">
-        <v>43053</v>
+        <v>35313</v>
       </c>
       <c r="B33">
-        <v>2017</v>
+        <v>1996</v>
       </c>
       <c r="C33">
-        <v>2.54573700790961</v>
+        <v>1.335102954533496</v>
       </c>
       <c r="D33">
-        <v>2018</v>
+        <v>1997</v>
       </c>
       <c r="E33">
-        <v>2.15356679889549</v>
+        <v>2.984773230892523</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2">
+        <v>35403</v>
+      </c>
+      <c r="B34">
+        <v>1996</v>
+      </c>
+      <c r="C34">
+        <v>1.482055350913747</v>
+      </c>
+      <c r="D34">
+        <v>1997</v>
+      </c>
+      <c r="E34">
+        <v>2.992107960012036</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2">
+        <v>35493</v>
+      </c>
+      <c r="B35">
+        <v>1997</v>
+      </c>
+      <c r="C35">
+        <v>2.445312678728806</v>
+      </c>
+      <c r="D35">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2">
+        <v>35586</v>
+      </c>
+      <c r="B36">
+        <v>1997</v>
+      </c>
+      <c r="C36">
+        <v>2.220119463330095</v>
+      </c>
+      <c r="D36">
+        <v>1998</v>
+      </c>
+      <c r="E36">
+        <v>2.64319810490059</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2">
+        <v>35683</v>
+      </c>
+      <c r="B37">
+        <v>1997</v>
+      </c>
+      <c r="C37">
+        <v>2.342165263381912</v>
+      </c>
+      <c r="D37">
+        <v>1998</v>
+      </c>
+      <c r="E37">
+        <v>2.716886837551424</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2">
+        <v>35768</v>
+      </c>
+      <c r="B38">
+        <v>1997</v>
+      </c>
+      <c r="C38">
+        <v>2.439884175301343</v>
+      </c>
+      <c r="D38">
+        <v>1998</v>
+      </c>
+      <c r="E38">
+        <v>2.773863658824549</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2">
+        <v>35881</v>
+      </c>
+      <c r="B39">
+        <v>1998</v>
+      </c>
+      <c r="C39">
+        <v>2.381150117272068</v>
+      </c>
+      <c r="D39">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2">
+        <v>35950</v>
+      </c>
+      <c r="B40">
+        <v>1998</v>
+      </c>
+      <c r="C40">
+        <v>2.772784171603737</v>
+      </c>
+      <c r="D40">
+        <v>1999</v>
+      </c>
+      <c r="E40">
+        <v>2.689796511187437</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2">
+        <v>36047</v>
+      </c>
+      <c r="B41">
+        <v>1998</v>
+      </c>
+      <c r="C41">
+        <v>2.84227685047822</v>
+      </c>
+      <c r="D41">
+        <v>1999</v>
+      </c>
+      <c r="E41">
+        <v>2.469054913123125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2">
+        <v>36132</v>
+      </c>
+      <c r="B42">
+        <v>1998</v>
+      </c>
+      <c r="C42">
+        <v>2.833473913903406</v>
+      </c>
+      <c r="D42">
+        <v>1999</v>
+      </c>
+      <c r="E42">
+        <v>2.482507310682891</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="2">
+        <v>36223</v>
+      </c>
+      <c r="B43">
+        <v>1999</v>
+      </c>
+      <c r="C43">
+        <v>1.655287196880928</v>
+      </c>
+      <c r="D43">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="2">
+        <v>36319</v>
+      </c>
+      <c r="B44">
+        <v>1999</v>
+      </c>
+      <c r="C44">
+        <v>1.481562820846571</v>
+      </c>
+      <c r="D44">
+        <v>2000</v>
+      </c>
+      <c r="E44">
+        <v>2.564763317404561</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="2">
+        <v>36412</v>
+      </c>
+      <c r="B45">
+        <v>1999</v>
+      </c>
+      <c r="C45">
+        <v>0.8861546371220719</v>
+      </c>
+      <c r="D45">
+        <v>2000</v>
+      </c>
+      <c r="E45">
+        <v>2.142429114246314</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="2">
+        <v>36501</v>
+      </c>
+      <c r="B46">
+        <v>1999</v>
+      </c>
+      <c r="C46">
+        <v>1.221733233617339</v>
+      </c>
+      <c r="D46">
+        <v>2000</v>
+      </c>
+      <c r="E46">
+        <v>2.282946612411263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="2">
+        <v>36587</v>
+      </c>
+      <c r="B47">
+        <v>2000</v>
+      </c>
+      <c r="C47">
+        <v>2.448320502468238</v>
+      </c>
+      <c r="D47">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2">
+        <v>36676</v>
+      </c>
+      <c r="B48">
+        <v>2000</v>
+      </c>
+      <c r="C48">
+        <v>2.564024492763806</v>
+      </c>
+      <c r="D48">
+        <v>2001</v>
+      </c>
+      <c r="E48">
+        <v>2.473062944816595</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2">
+        <v>36767</v>
+      </c>
+      <c r="B49">
+        <v>2000</v>
+      </c>
+      <c r="C49">
+        <v>3.153099622684863</v>
+      </c>
+      <c r="D49">
+        <v>2001</v>
+      </c>
+      <c r="E49">
+        <v>2.621515653474216</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="2">
+        <v>36858</v>
+      </c>
+      <c r="B50">
+        <v>2000</v>
+      </c>
+      <c r="C50">
+        <v>3.212706544592092</v>
+      </c>
+      <c r="D50">
+        <v>2001</v>
+      </c>
+      <c r="E50">
+        <v>2.498927718860466</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2">
+        <v>36951</v>
+      </c>
+      <c r="B51">
+        <v>2001</v>
+      </c>
+      <c r="C51">
+        <v>1.915232257141031</v>
+      </c>
+      <c r="D51">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2">
+        <v>37034</v>
+      </c>
+      <c r="B52">
+        <v>2001</v>
+      </c>
+      <c r="C52">
+        <v>1.759737107832926</v>
+      </c>
+      <c r="D52">
+        <v>2002</v>
+      </c>
+      <c r="E52">
+        <v>2.1823787252363</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2">
+        <v>37126</v>
+      </c>
+      <c r="B53">
+        <v>2001</v>
+      </c>
+      <c r="C53">
+        <v>1.200212790305688</v>
+      </c>
+      <c r="D53">
+        <v>2002</v>
+      </c>
+      <c r="E53">
+        <v>1.945361731599915</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2">
+        <v>37222</v>
+      </c>
+      <c r="B54">
+        <v>2001</v>
+      </c>
+      <c r="C54">
+        <v>0.8718408608820116</v>
+      </c>
+      <c r="D54">
+        <v>2002</v>
+      </c>
+      <c r="E54">
+        <v>1.451589658605279</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2">
+        <v>37314</v>
+      </c>
+      <c r="B55">
+        <v>2002</v>
+      </c>
+      <c r="C55">
+        <v>0.7448884326621386</v>
+      </c>
+      <c r="D55">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="2">
+        <v>37399</v>
+      </c>
+      <c r="B56">
+        <v>2002</v>
+      </c>
+      <c r="C56">
+        <v>0.5027243209395182</v>
+      </c>
+      <c r="D56">
+        <v>2003</v>
+      </c>
+      <c r="E56">
+        <v>1.723557921614716</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="2">
+        <v>37490</v>
+      </c>
+      <c r="B57">
+        <v>2002</v>
+      </c>
+      <c r="C57">
+        <v>0.4808578657098828</v>
+      </c>
+      <c r="D57">
+        <v>2003</v>
+      </c>
+      <c r="E57">
+        <v>1.723271795704595</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2">
+        <v>37581</v>
+      </c>
+      <c r="B58">
+        <v>2002</v>
+      </c>
+      <c r="C58">
+        <v>0.3027105478702108</v>
+      </c>
+      <c r="D58">
+        <v>2003</v>
+      </c>
+      <c r="E58">
+        <v>1.495147488490889</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="2">
+        <v>37678</v>
+      </c>
+      <c r="B59">
+        <v>2003</v>
+      </c>
+      <c r="C59">
+        <v>1.101570631429216</v>
+      </c>
+      <c r="D59">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2">
+        <v>37756</v>
+      </c>
+      <c r="B60">
+        <v>2003</v>
+      </c>
+      <c r="C60">
+        <v>0.5465690596114792</v>
+      </c>
+      <c r="D60">
+        <v>2004</v>
+      </c>
+      <c r="E60">
+        <v>1.336255717893819</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2">
+        <v>37847</v>
+      </c>
+      <c r="B61">
+        <v>2003</v>
+      </c>
+      <c r="C61">
+        <v>0.1226244738887772</v>
+      </c>
+      <c r="D61">
+        <v>2004</v>
+      </c>
+      <c r="E61">
+        <v>1.273847785608018</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2">
+        <v>37938</v>
+      </c>
+      <c r="B62">
+        <v>2003</v>
+      </c>
+      <c r="C62">
+        <v>-0.06338401458176879</v>
+      </c>
+      <c r="D62">
+        <v>2004</v>
+      </c>
+      <c r="E62">
+        <v>1.186949455574493</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2">
+        <v>38029</v>
+      </c>
+      <c r="B63">
+        <v>2004</v>
+      </c>
+      <c r="C63">
+        <v>0.995052798292595</v>
+      </c>
+      <c r="D63">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2">
+        <v>38120</v>
+      </c>
+      <c r="B64">
+        <v>2004</v>
+      </c>
+      <c r="C64">
+        <v>1.097102853016874</v>
+      </c>
+      <c r="D64">
+        <v>2005</v>
+      </c>
+      <c r="E64">
+        <v>1.078165363345507</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="2">
+        <v>38211</v>
+      </c>
+      <c r="B65">
+        <v>2004</v>
+      </c>
+      <c r="C65">
+        <v>1.34901080838441</v>
+      </c>
+      <c r="D65">
+        <v>2005</v>
+      </c>
+      <c r="E65">
+        <v>1.284205480024792</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="2">
+        <v>38302</v>
+      </c>
+      <c r="B66">
+        <v>2004</v>
+      </c>
+      <c r="C66">
+        <v>1.191718234579842</v>
+      </c>
+      <c r="D66">
+        <v>2005</v>
+      </c>
+      <c r="E66">
+        <v>1.166653268907458</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="2">
+        <v>38398</v>
+      </c>
+      <c r="B67">
+        <v>2005</v>
+      </c>
+      <c r="C67">
+        <v>0.5395053573269193</v>
+      </c>
+      <c r="D67">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="2">
+        <v>38484</v>
+      </c>
+      <c r="B68">
+        <v>2005</v>
+      </c>
+      <c r="C68">
+        <v>1.572397351130328</v>
+      </c>
+      <c r="D68">
+        <v>2006</v>
+      </c>
+      <c r="E68">
+        <v>1.582707465349764</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="2">
+        <v>38575</v>
+      </c>
+      <c r="B69">
+        <v>2005</v>
+      </c>
+      <c r="C69">
+        <v>0.9830139229099144</v>
+      </c>
+      <c r="D69">
+        <v>2006</v>
+      </c>
+      <c r="E69">
+        <v>1.422422035968962</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="2">
+        <v>38671</v>
+      </c>
+      <c r="B70">
+        <v>2005</v>
+      </c>
+      <c r="C70">
+        <v>1.10662279082161</v>
+      </c>
+      <c r="D70">
+        <v>2006</v>
+      </c>
+      <c r="E70">
+        <v>1.607604296724396</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="2">
+        <v>38762</v>
+      </c>
+      <c r="B71">
+        <v>2006</v>
+      </c>
+      <c r="C71">
+        <v>1.321777562372928</v>
+      </c>
+      <c r="D71">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="2">
+        <v>38848</v>
+      </c>
+      <c r="B72">
+        <v>2006</v>
+      </c>
+      <c r="C72">
+        <v>1.322125352849413</v>
+      </c>
+      <c r="D72">
+        <v>2007</v>
+      </c>
+      <c r="E72">
+        <v>1.429193111889671</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="2">
+        <v>38943</v>
+      </c>
+      <c r="B73">
+        <v>2006</v>
+      </c>
+      <c r="C73">
+        <v>2.206144542976007</v>
+      </c>
+      <c r="D73">
+        <v>2007</v>
+      </c>
+      <c r="E73">
+        <v>1.674846040945321</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="2">
+        <v>39035</v>
+      </c>
+      <c r="B74">
+        <v>2006</v>
+      </c>
+      <c r="C74">
+        <v>2.581733062021807</v>
+      </c>
+      <c r="D74">
+        <v>2007</v>
+      </c>
+      <c r="E74">
+        <v>1.863208987134324</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="2">
+        <v>39126</v>
+      </c>
+      <c r="B75">
+        <v>2007</v>
+      </c>
+      <c r="C75">
+        <v>2.416268882941885</v>
+      </c>
+      <c r="D75">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="2">
+        <v>39217</v>
+      </c>
+      <c r="B76">
+        <v>2007</v>
+      </c>
+      <c r="C76">
+        <v>2.644331987985127</v>
+      </c>
+      <c r="D76">
+        <v>2008</v>
+      </c>
+      <c r="E76">
+        <v>1.618758147029653</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="2">
+        <v>39308</v>
+      </c>
+      <c r="B77">
+        <v>2007</v>
+      </c>
+      <c r="C77">
+        <v>2.463900898486049</v>
+      </c>
+      <c r="D77">
+        <v>2008</v>
+      </c>
+      <c r="E77">
+        <v>1.439039865002134</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="2">
+        <v>39400</v>
+      </c>
+      <c r="B78">
+        <v>2007</v>
+      </c>
+      <c r="C78">
+        <v>2.635105211127575</v>
+      </c>
+      <c r="D78">
+        <v>2008</v>
+      </c>
+      <c r="E78">
+        <v>1.722015618408701</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="2">
+        <v>39492</v>
+      </c>
+      <c r="B79">
+        <v>2008</v>
+      </c>
+      <c r="C79">
+        <v>1.585034188191714</v>
+      </c>
+      <c r="D79">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="2">
+        <v>39583</v>
+      </c>
+      <c r="B80">
+        <v>2008</v>
+      </c>
+      <c r="C80">
+        <v>2.914742198403797</v>
+      </c>
+      <c r="D80">
+        <v>2009</v>
+      </c>
+      <c r="E80">
+        <v>1.949882598369124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="2">
+        <v>39674</v>
+      </c>
+      <c r="B81">
+        <v>2008</v>
+      </c>
+      <c r="C81">
+        <v>1.849664159209219</v>
+      </c>
+      <c r="D81">
+        <v>2009</v>
+      </c>
+      <c r="E81">
+        <v>1.258622825501221</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="2">
+        <v>39765</v>
+      </c>
+      <c r="B82">
+        <v>2008</v>
+      </c>
+      <c r="C82">
+        <v>1.485199759936107</v>
+      </c>
+      <c r="D82">
+        <v>2009</v>
+      </c>
+      <c r="E82">
+        <v>0.443605991657714</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="2">
+        <v>39857</v>
+      </c>
+      <c r="B83">
+        <v>2009</v>
+      </c>
+      <c r="C83">
+        <v>-2.925220177089027</v>
+      </c>
+      <c r="D83">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="2">
+        <v>39948</v>
+      </c>
+      <c r="B84">
+        <v>2009</v>
+      </c>
+      <c r="C84">
+        <v>-10.38912473755519</v>
+      </c>
+      <c r="D84">
+        <v>2010</v>
+      </c>
+      <c r="E84">
+        <v>-13.02588630704915</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="2">
+        <v>40038</v>
+      </c>
+      <c r="B85">
+        <v>2009</v>
+      </c>
+      <c r="C85">
+        <v>-5.493279456187173</v>
+      </c>
+      <c r="D85">
+        <v>2010</v>
+      </c>
+      <c r="E85">
+        <v>0.3099897690161502</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="2">
+        <v>40130</v>
+      </c>
+      <c r="B86">
+        <v>2009</v>
+      </c>
+      <c r="C86">
+        <v>-4.838386464989386</v>
+      </c>
+      <c r="D86">
+        <v>2010</v>
+      </c>
+      <c r="E86">
+        <v>1.556350517939564</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="2">
+        <v>40221</v>
+      </c>
+      <c r="B87">
+        <v>2010</v>
+      </c>
+      <c r="C87">
+        <v>0.9288791585305711</v>
+      </c>
+      <c r="D87">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="2">
+        <v>40310</v>
+      </c>
+      <c r="B88">
+        <v>2010</v>
+      </c>
+      <c r="C88">
+        <v>1.071809041675276</v>
+      </c>
+      <c r="D88">
+        <v>2011</v>
+      </c>
+      <c r="E88">
+        <v>0.8342879232527967</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="2">
+        <v>40403</v>
+      </c>
+      <c r="B89">
+        <v>2010</v>
+      </c>
+      <c r="C89">
+        <v>3.577564492651675</v>
+      </c>
+      <c r="D89">
+        <v>2011</v>
+      </c>
+      <c r="E89">
+        <v>2.731583858664188</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="2">
+        <v>40494</v>
+      </c>
+      <c r="B90">
+        <v>2010</v>
+      </c>
+      <c r="C90">
+        <v>3.522877896197807</v>
+      </c>
+      <c r="D90">
+        <v>2011</v>
+      </c>
+      <c r="E90">
+        <v>2.252953350090348</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="2">
+        <v>40589</v>
+      </c>
+      <c r="B91">
+        <v>2011</v>
+      </c>
+      <c r="C91">
+        <v>2.021953894754303</v>
+      </c>
+      <c r="D91">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="2">
+        <v>40676</v>
+      </c>
+      <c r="B92">
+        <v>2011</v>
+      </c>
+      <c r="C92">
+        <v>3.720096369677184</v>
+      </c>
+      <c r="D92">
+        <v>2012</v>
+      </c>
+      <c r="E92">
+        <v>1.686787594525496</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="2">
+        <v>40771</v>
+      </c>
+      <c r="B93">
+        <v>2011</v>
+      </c>
+      <c r="C93">
+        <v>2.851982935378228</v>
+      </c>
+      <c r="D93">
+        <v>2012</v>
+      </c>
+      <c r="E93">
+        <v>1.136030550102829</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="2">
+        <v>40862</v>
+      </c>
+      <c r="B94">
+        <v>2011</v>
+      </c>
+      <c r="C94">
+        <v>3.172593145981373</v>
+      </c>
+      <c r="D94">
+        <v>2012</v>
+      </c>
+      <c r="E94">
+        <v>1.460171959067247</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="2">
+        <v>40954</v>
+      </c>
+      <c r="B95">
+        <v>2012</v>
+      </c>
+      <c r="C95">
+        <v>0.613364121638349</v>
+      </c>
+      <c r="D95">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="2">
+        <v>41044</v>
+      </c>
+      <c r="B96">
+        <v>2012</v>
+      </c>
+      <c r="C96">
+        <v>1.276650241283095</v>
+      </c>
+      <c r="D96">
+        <v>2013</v>
+      </c>
+      <c r="E96">
+        <v>1.19633550657503</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="2">
+        <v>41135</v>
+      </c>
+      <c r="B97">
+        <v>2012</v>
+      </c>
+      <c r="C97">
+        <v>1.086563863520862</v>
+      </c>
+      <c r="D97">
+        <v>2013</v>
+      </c>
+      <c r="E97">
+        <v>1.06457164149647</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="2">
+        <v>41228</v>
+      </c>
+      <c r="B98">
+        <v>2012</v>
+      </c>
+      <c r="C98">
+        <v>1.075749333634834</v>
+      </c>
+      <c r="D98">
+        <v>2013</v>
+      </c>
+      <c r="E98">
+        <v>1.106002658655192</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="2">
+        <v>41319</v>
+      </c>
+      <c r="B99">
+        <v>2013</v>
+      </c>
+      <c r="C99">
+        <v>-0.1408840671955125</v>
+      </c>
+      <c r="D99">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="2">
+        <v>41409</v>
+      </c>
+      <c r="B100">
+        <v>2013</v>
+      </c>
+      <c r="C100">
+        <v>-0.03137857138646449</v>
+      </c>
+      <c r="D100">
+        <v>2014</v>
+      </c>
+      <c r="E100">
+        <v>0.8494291553396094</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="2">
+        <v>41500</v>
+      </c>
+      <c r="B101">
+        <v>2013</v>
+      </c>
+      <c r="C101">
+        <v>0.6094282583182231</v>
+      </c>
+      <c r="D101">
+        <v>2014</v>
+      </c>
+      <c r="E101">
+        <v>1.440500538214629</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="2">
+        <v>41592</v>
+      </c>
+      <c r="B102">
+        <v>2013</v>
+      </c>
+      <c r="C102">
+        <v>0.5135943516859198</v>
+      </c>
+      <c r="D102">
+        <v>2014</v>
+      </c>
+      <c r="E102">
+        <v>1.304915753449687</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="2">
+        <v>41684</v>
+      </c>
+      <c r="B103">
+        <v>2014</v>
+      </c>
+      <c r="C103">
+        <v>1.408749482567595</v>
+      </c>
+      <c r="D103">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="2">
+        <v>41774</v>
+      </c>
+      <c r="B104">
+        <v>2014</v>
+      </c>
+      <c r="C104">
+        <v>2.183348446776856</v>
+      </c>
+      <c r="D104">
+        <v>2015</v>
+      </c>
+      <c r="E104">
+        <v>1.476241482808471</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="2">
+        <v>41865</v>
+      </c>
+      <c r="B105">
+        <v>2014</v>
+      </c>
+      <c r="C105">
+        <v>1.308305381840369</v>
+      </c>
+      <c r="D105">
+        <v>2015</v>
+      </c>
+      <c r="E105">
+        <v>0.726330085526028</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="2">
+        <v>41957</v>
+      </c>
+      <c r="B106">
+        <v>2014</v>
+      </c>
+      <c r="C106">
+        <v>1.463603839062211</v>
+      </c>
+      <c r="D106">
+        <v>2015</v>
+      </c>
+      <c r="E106">
+        <v>0.7345358670387547</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="2">
+        <v>42048</v>
+      </c>
+      <c r="B107">
+        <v>2015</v>
+      </c>
+      <c r="C107">
+        <v>1.555506802213324</v>
+      </c>
+      <c r="D107">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="2">
+        <v>42137</v>
+      </c>
+      <c r="B108">
+        <v>2015</v>
+      </c>
+      <c r="C108">
+        <v>1.291204709804039</v>
+      </c>
+      <c r="D108">
+        <v>2016</v>
+      </c>
+      <c r="E108">
+        <v>1.334784545494694</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="2">
+        <v>42230</v>
+      </c>
+      <c r="B109">
+        <v>2015</v>
+      </c>
+      <c r="C109">
+        <v>1.503879794234519</v>
+      </c>
+      <c r="D109">
+        <v>2016</v>
+      </c>
+      <c r="E109">
+        <v>1.427154289074717</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="2">
+        <v>42321</v>
+      </c>
+      <c r="B110">
+        <v>2015</v>
+      </c>
+      <c r="C110">
+        <v>1.460561192715071</v>
+      </c>
+      <c r="D110">
+        <v>2016</v>
+      </c>
+      <c r="E110">
+        <v>1.316306168565684</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="2">
+        <v>42412</v>
+      </c>
+      <c r="B111">
+        <v>2016</v>
+      </c>
+      <c r="C111">
+        <v>1.211140135558786</v>
+      </c>
+      <c r="D111">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="2">
+        <v>42503</v>
+      </c>
+      <c r="B112">
+        <v>2016</v>
+      </c>
+      <c r="C112">
+        <v>1.789277221144991</v>
+      </c>
+      <c r="D112">
+        <v>2017</v>
+      </c>
+      <c r="E112">
+        <v>1.517762585655458</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="2">
+        <v>42594</v>
+      </c>
+      <c r="B113">
+        <v>2016</v>
+      </c>
+      <c r="C113">
+        <v>1.831409032854858</v>
+      </c>
+      <c r="D113">
+        <v>2017</v>
+      </c>
+      <c r="E113">
+        <v>1.455762792597137</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="2">
+        <v>42689</v>
+      </c>
+      <c r="B114">
+        <v>2016</v>
+      </c>
+      <c r="C114">
+        <v>1.71486702353103</v>
+      </c>
+      <c r="D114">
+        <v>2017</v>
+      </c>
+      <c r="E114">
+        <v>1.271337706785514</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="2">
+        <v>42780</v>
+      </c>
+      <c r="B115">
+        <v>2017</v>
+      </c>
+      <c r="C115">
+        <v>1.469790059051301</v>
+      </c>
+      <c r="D115">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="2">
+        <v>42867</v>
+      </c>
+      <c r="B116">
+        <v>2017</v>
+      </c>
+      <c r="C116">
+        <v>1.816297695264346</v>
+      </c>
+      <c r="D116">
+        <v>2018</v>
+      </c>
+      <c r="E116">
+        <v>1.651160881705249</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="2">
+        <v>42962</v>
+      </c>
+      <c r="B117">
+        <v>2017</v>
+      </c>
+      <c r="C117">
+        <v>2.141958087655205</v>
+      </c>
+      <c r="D117">
+        <v>2018</v>
+      </c>
+      <c r="E117">
+        <v>1.746314025496809</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="2">
+        <v>43053</v>
+      </c>
+      <c r="B118">
+        <v>2017</v>
+      </c>
+      <c r="C118">
+        <v>2.54573700790961</v>
+      </c>
+      <c r="D118">
+        <v>2018</v>
+      </c>
+      <c r="E118">
+        <v>2.15356679889549</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="2">
         <v>43145</v>
       </c>
-      <c r="B34">
+      <c r="B119">
         <v>2018</v>
       </c>
-      <c r="C34">
+      <c r="C119">
         <v>2.145682023461037</v>
       </c>
-      <c r="D34">
+      <c r="D119">
         <v>2019</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="2">
+        <v>43235</v>
+      </c>
+      <c r="B120">
+        <v>2018</v>
+      </c>
+      <c r="C120">
+        <v>1.814946630842762</v>
+      </c>
+      <c r="D120">
+        <v>2019</v>
+      </c>
+      <c r="E120">
+        <v>1.477668145972499</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="2">
+        <v>43326</v>
+      </c>
+      <c r="B121">
+        <v>2018</v>
+      </c>
+      <c r="C121">
+        <v>1.833917811424923</v>
+      </c>
+      <c r="D121">
+        <v>2019</v>
+      </c>
+      <c r="E121">
+        <v>1.482713323460105</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="2">
+        <v>43418</v>
+      </c>
+      <c r="B122">
+        <v>2018</v>
+      </c>
+      <c r="C122">
+        <v>1.467563812511452</v>
+      </c>
+      <c r="D122">
+        <v>2019</v>
+      </c>
+      <c r="E122">
+        <v>0.7694605565311097</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="2">
+        <v>43510</v>
+      </c>
+      <c r="B123">
+        <v>2019</v>
+      </c>
+      <c r="C123">
+        <v>0.6144150995606168</v>
+      </c>
+      <c r="D123">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="2">
+        <v>43600</v>
+      </c>
+      <c r="B124">
+        <v>2019</v>
+      </c>
+      <c r="C124">
+        <v>0.9755302942728195</v>
+      </c>
+      <c r="D124">
+        <v>2020</v>
+      </c>
+      <c r="E124">
+        <v>1.308311503751969</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="2">
+        <v>43691</v>
+      </c>
+      <c r="B125">
+        <v>2019</v>
+      </c>
+      <c r="C125">
+        <v>0.6763657625222574</v>
+      </c>
+      <c r="D125">
+        <v>2020</v>
+      </c>
+      <c r="E125">
+        <v>0.9449343475431693</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="2">
+        <v>43783</v>
+      </c>
+      <c r="B126">
+        <v>2019</v>
+      </c>
+      <c r="C126">
+        <v>0.573813583266336</v>
+      </c>
+      <c r="D126">
+        <v>2020</v>
+      </c>
+      <c r="E126">
+        <v>0.7682770484317203</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="2">
+        <v>43875</v>
+      </c>
+      <c r="B127">
+        <v>2020</v>
+      </c>
+      <c r="C127">
+        <v>0.6190211190723716</v>
+      </c>
+      <c r="D127">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="2">
+        <v>43966</v>
+      </c>
+      <c r="B128">
+        <v>2020</v>
+      </c>
+      <c r="C128">
+        <v>-2.88765784846251</v>
+      </c>
+      <c r="D128">
+        <v>2021</v>
+      </c>
+      <c r="E128">
+        <v>-0.08203399280549695</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B129">
+        <v>2020</v>
+      </c>
+      <c r="C129">
+        <v>-13.62257802198732</v>
+      </c>
+      <c r="D129">
+        <v>2021</v>
+      </c>
+      <c r="E129">
+        <v>-18.77753932536402</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="2">
+        <v>44159</v>
+      </c>
+      <c r="B130">
+        <v>2020</v>
+      </c>
+      <c r="C130">
+        <v>-6.332038390823524</v>
+      </c>
+      <c r="D130">
+        <v>2021</v>
+      </c>
+      <c r="E130">
+        <v>0.4447691747926807</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="2">
+        <v>44251</v>
+      </c>
+      <c r="B131">
+        <v>2021</v>
+      </c>
+      <c r="C131">
+        <v>1.393690305272322</v>
+      </c>
+      <c r="D131">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="2">
+        <v>44341</v>
+      </c>
+      <c r="B132">
+        <v>2021</v>
+      </c>
+      <c r="C132">
+        <v>1.10051964147142</v>
+      </c>
+      <c r="D132">
+        <v>2022</v>
+      </c>
+      <c r="E132">
+        <v>1.367775147972683</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="2">
+        <v>44432</v>
+      </c>
+      <c r="B133">
+        <v>2021</v>
+      </c>
+      <c r="C133">
+        <v>1.596719456215823</v>
+      </c>
+      <c r="D133">
+        <v>2022</v>
+      </c>
+      <c r="E133">
+        <v>1.64009848016855</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" s="2">
+        <v>44525</v>
+      </c>
+      <c r="B134">
+        <v>2021</v>
+      </c>
+      <c r="C134">
+        <v>2.50078376310503</v>
+      </c>
+      <c r="D134">
+        <v>2022</v>
+      </c>
+      <c r="E134">
+        <v>2.02294041918627</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" s="2">
+        <v>44617</v>
+      </c>
+      <c r="B135">
+        <v>2022</v>
+      </c>
+      <c r="C135">
+        <v>2.171220559958353</v>
+      </c>
+      <c r="D135">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" s="2">
+        <v>44706</v>
+      </c>
+      <c r="B136">
+        <v>2022</v>
+      </c>
+      <c r="C136">
+        <v>2.093637744778643</v>
+      </c>
+      <c r="D136">
+        <v>2023</v>
+      </c>
+      <c r="E136">
+        <v>1.595534183633029</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" s="2">
+        <v>44798</v>
+      </c>
+      <c r="B137">
+        <v>2022</v>
+      </c>
+      <c r="C137">
+        <v>2.047503765332293</v>
+      </c>
+      <c r="D137">
+        <v>2023</v>
+      </c>
+      <c r="E137">
+        <v>1.450008929318436</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="2">
+        <v>44890</v>
+      </c>
+      <c r="B138">
+        <v>2022</v>
+      </c>
+      <c r="C138">
+        <v>2.036925251458377</v>
+      </c>
+      <c r="D138">
+        <v>2023</v>
+      </c>
+      <c r="E138">
+        <v>1.390457834055581</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="2">
+        <v>44981</v>
+      </c>
+      <c r="B139">
+        <v>2023</v>
+      </c>
+      <c r="C139">
+        <v>1.094238427434013</v>
+      </c>
+      <c r="D139">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="2">
+        <v>45071</v>
+      </c>
+      <c r="B140">
+        <v>2023</v>
+      </c>
+      <c r="C140">
+        <v>0.2704008632326893</v>
+      </c>
+      <c r="D140">
+        <v>2024</v>
+      </c>
+      <c r="E140">
+        <v>1.264914507337878</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="2">
+        <v>45163</v>
+      </c>
+      <c r="B141">
+        <v>2023</v>
+      </c>
+      <c r="C141">
+        <v>0.0973275205688573</v>
+      </c>
+      <c r="D141">
+        <v>2024</v>
+      </c>
+      <c r="E141">
+        <v>1.155931536963561</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="2">
+        <v>45254</v>
+      </c>
+      <c r="B142">
+        <v>2023</v>
+      </c>
+      <c r="C142">
+        <v>0.006976824310989116</v>
+      </c>
+      <c r="D142">
+        <v>2024</v>
+      </c>
+      <c r="E142">
+        <v>1.013493932837783</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="2">
+        <v>45345</v>
+      </c>
+      <c r="B143">
+        <v>2024</v>
+      </c>
+      <c r="C143">
+        <v>0.777040352969971</v>
+      </c>
+      <c r="D143">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="2">
+        <v>45436</v>
+      </c>
+      <c r="B144">
+        <v>2024</v>
+      </c>
+      <c r="C144">
+        <v>0.4339626597083202</v>
+      </c>
+      <c r="D144">
+        <v>2025</v>
+      </c>
+      <c r="E144">
+        <v>1.098925859512323</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="2">
+        <v>45534</v>
+      </c>
+      <c r="B145">
+        <v>2024</v>
+      </c>
+      <c r="C145">
+        <v>0.233555755601067</v>
+      </c>
+      <c r="D145">
+        <v>2025</v>
+      </c>
+      <c r="E145">
+        <v>1.030082119929365</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="2">
+        <v>45618</v>
+      </c>
+      <c r="B146">
+        <v>2024</v>
+      </c>
+      <c r="C146">
+        <v>-0.03686848375263896</v>
+      </c>
+      <c r="D146">
+        <v>2025</v>
+      </c>
+      <c r="E146">
+        <v>0.9237465935730382</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="2">
+        <v>45713</v>
+      </c>
+      <c r="B147">
+        <v>2025</v>
+      </c>
+      <c r="C147">
+        <v>0.6896020733472286</v>
+      </c>
+      <c r="D147">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="2">
+        <v>45800</v>
+      </c>
+      <c r="B148">
+        <v>2025</v>
+      </c>
+      <c r="C148">
+        <v>0.6712205726778775</v>
+      </c>
+      <c r="D148">
+        <v>2026</v>
+      </c>
+      <c r="E148">
+        <v>1.081926859399074</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="2">
+        <v>45891</v>
+      </c>
+      <c r="B149">
+        <v>2025</v>
+      </c>
+      <c r="C149">
+        <v>0.4755036192378936</v>
+      </c>
+      <c r="D149">
+        <v>2026</v>
+      </c>
+      <c r="E149">
+        <v>0.9694102959983519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>